<commit_message>
Version 1.1 - Change figures to show amount GAVI co-financed instead of proportion (GAVI co-financing data does not match CEA data for several resons) - Added Yellow fever CEA to data - Changed figure formatting - Added figures
</commit_message>
<xml_diff>
--- a/data/Data18032020.xlsx
+++ b/data/Data18032020.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\btb15109\OneDrive\Work\Project\GHD DFID iDSI\DonorModel\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eae25fc990f688b4/Work/Project/GHD DFID iDSI/Vaccine-Co-financing-Model/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27315" windowHeight="15360" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27315" windowHeight="15360" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GDP per capita_at current Price" sheetId="2" r:id="rId1"/>
     <sheet name="GDP per capita_at PPP" sheetId="4" r:id="rId2"/>
-    <sheet name="CEA_new" sheetId="7" r:id="rId3"/>
+    <sheet name="data_cea" sheetId="7" r:id="rId3"/>
     <sheet name="Cost Burden1" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="94">
   <si>
     <t>Country</t>
   </si>
@@ -1601,13 +1601,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X109"/>
+  <dimension ref="A1:X112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D59" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="I8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A102" sqref="A102:C105"/>
+      <selection pane="bottomRight" activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1693,7 +1693,7 @@
         <v>18621.8</v>
       </c>
       <c r="H2" s="25">
-        <f t="shared" ref="H2:H33" si="0">E2/G2</f>
+        <f t="shared" ref="H2:H36" si="0">E2/G2</f>
         <v>80.849821177329801</v>
       </c>
       <c r="I2" s="23">
@@ -2902,25 +2902,25 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="23" t="s">
-        <v>88</v>
+        <v>6</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C33" s="23" t="s">
         <v>35</v>
       </c>
       <c r="D33" s="24"/>
-      <c r="E33" s="24">
-        <v>911814</v>
+      <c r="E33" s="2">
+        <v>1197317</v>
       </c>
       <c r="F33" s="24"/>
-      <c r="G33" s="26">
-        <v>19188</v>
-      </c>
-      <c r="H33" s="25">
-        <f t="shared" si="0"/>
-        <v>47.520012507817384</v>
+      <c r="G33">
+        <v>4942</v>
+      </c>
+      <c r="H33" s="11">
+        <f>E33/G33</f>
+        <v>242.27377579927156</v>
       </c>
       <c r="I33" s="23"/>
       <c r="J33" s="23"/>
@@ -2937,25 +2937,25 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="23" t="s">
-        <v>88</v>
+        <v>6</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C34" s="23" t="s">
         <v>21</v>
       </c>
       <c r="D34" s="24"/>
-      <c r="E34" s="24">
-        <v>911814</v>
+      <c r="E34" s="2">
+        <v>1197317</v>
       </c>
       <c r="F34" s="24"/>
-      <c r="G34" s="26">
-        <v>216</v>
-      </c>
-      <c r="H34" s="25">
-        <f t="shared" ref="H34:H65" si="1">E34/G34</f>
-        <v>4221.3611111111113</v>
+      <c r="G34">
+        <v>745</v>
+      </c>
+      <c r="H34" s="11">
+        <f>E34/G34</f>
+        <v>1607.1369127516778</v>
       </c>
       <c r="I34" s="23"/>
       <c r="J34" s="23"/>
@@ -2972,25 +2972,25 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B35" s="23" t="s">
-        <v>88</v>
+        <v>6</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C35" s="23" t="s">
         <v>39</v>
       </c>
       <c r="D35" s="24"/>
-      <c r="E35" s="24">
-        <v>911814</v>
+      <c r="E35" s="2">
+        <v>1197317</v>
       </c>
       <c r="F35" s="24"/>
-      <c r="G35" s="26">
-        <v>8624</v>
-      </c>
-      <c r="H35" s="25">
-        <f t="shared" si="1"/>
-        <v>105.7298237476809</v>
+      <c r="G35">
+        <v>26855</v>
+      </c>
+      <c r="H35" s="11">
+        <f>E35/G35</f>
+        <v>44.58450940234593</v>
       </c>
       <c r="I35" s="23"/>
       <c r="J35" s="23"/>
@@ -3010,22 +3010,22 @@
         <v>40</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C36" s="23" t="s">
         <v>35</v>
       </c>
       <c r="D36" s="24"/>
       <c r="E36" s="24">
-        <v>302387</v>
+        <v>911814</v>
       </c>
       <c r="F36" s="24"/>
       <c r="G36" s="26">
-        <v>41</v>
+        <v>19188</v>
       </c>
       <c r="H36" s="25">
-        <f t="shared" si="1"/>
-        <v>7375.292682926829</v>
+        <f t="shared" si="0"/>
+        <v>47.520012507817384</v>
       </c>
       <c r="I36" s="23"/>
       <c r="J36" s="23"/>
@@ -3045,22 +3045,22 @@
         <v>40</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C37" s="23" t="s">
         <v>21</v>
       </c>
       <c r="D37" s="24"/>
       <c r="E37" s="24">
-        <v>302387</v>
+        <v>911814</v>
       </c>
       <c r="F37" s="24"/>
       <c r="G37" s="26">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="H37" s="25">
-        <f t="shared" si="1"/>
-        <v>33598.555555555555</v>
+        <f t="shared" ref="H37:H58" si="1">E37/G37</f>
+        <v>4221.3611111111113</v>
       </c>
       <c r="I37" s="23"/>
       <c r="J37" s="23"/>
@@ -3080,22 +3080,22 @@
         <v>40</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C38" s="23" t="s">
         <v>39</v>
       </c>
       <c r="D38" s="24"/>
       <c r="E38" s="24">
-        <v>302387</v>
+        <v>911814</v>
       </c>
       <c r="F38" s="24"/>
       <c r="G38" s="26">
-        <v>293</v>
+        <v>8624</v>
       </c>
       <c r="H38" s="25">
         <f t="shared" si="1"/>
-        <v>1032.037542662116</v>
+        <v>105.7298237476809</v>
       </c>
       <c r="I38" s="23"/>
       <c r="J38" s="23"/>
@@ -3115,22 +3115,22 @@
         <v>40</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C39" s="23" t="s">
         <v>35</v>
       </c>
       <c r="D39" s="24"/>
       <c r="E39" s="24">
-        <v>2190061</v>
+        <v>302387</v>
       </c>
       <c r="F39" s="24"/>
       <c r="G39" s="26">
-        <v>79582</v>
+        <v>41</v>
       </c>
       <c r="H39" s="25">
         <f t="shared" si="1"/>
-        <v>27.519552160036188</v>
+        <v>7375.292682926829</v>
       </c>
       <c r="I39" s="23"/>
       <c r="J39" s="23"/>
@@ -3150,22 +3150,22 @@
         <v>40</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C40" s="23" t="s">
         <v>21</v>
       </c>
       <c r="D40" s="24"/>
       <c r="E40" s="24">
-        <v>2190061</v>
+        <v>302387</v>
       </c>
       <c r="F40" s="24"/>
       <c r="G40" s="26">
-        <v>915</v>
+        <v>9</v>
       </c>
       <c r="H40" s="25">
         <f t="shared" si="1"/>
-        <v>2393.5092896174865</v>
+        <v>33598.555555555555</v>
       </c>
       <c r="I40" s="23"/>
       <c r="J40" s="23"/>
@@ -3185,22 +3185,22 @@
         <v>40</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C41" s="23" t="s">
         <v>39</v>
       </c>
       <c r="D41" s="24"/>
       <c r="E41" s="24">
-        <v>2190061</v>
+        <v>302387</v>
       </c>
       <c r="F41" s="24"/>
       <c r="G41" s="26">
-        <v>32112</v>
+        <v>293</v>
       </c>
       <c r="H41" s="25">
         <f t="shared" si="1"/>
-        <v>68.200703786746388</v>
+        <v>1032.037542662116</v>
       </c>
       <c r="I41" s="23"/>
       <c r="J41" s="23"/>
@@ -3217,25 +3217,25 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C42" s="23" t="s">
         <v>35</v>
       </c>
       <c r="D42" s="24"/>
       <c r="E42" s="24">
-        <v>2145697</v>
+        <v>2190061</v>
       </c>
       <c r="F42" s="24"/>
       <c r="G42" s="26">
-        <v>187887</v>
+        <v>79582</v>
       </c>
       <c r="H42" s="25">
         <f t="shared" si="1"/>
-        <v>11.420146151676274</v>
+        <v>27.519552160036188</v>
       </c>
       <c r="I42" s="23"/>
       <c r="J42" s="23"/>
@@ -3252,25 +3252,25 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C43" s="23" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="24"/>
       <c r="E43" s="24">
-        <v>2145697</v>
+        <v>2190061</v>
       </c>
       <c r="F43" s="24"/>
       <c r="G43" s="26">
-        <v>1615</v>
+        <v>915</v>
       </c>
       <c r="H43" s="25">
         <f t="shared" si="1"/>
-        <v>1328.6049535603715</v>
+        <v>2393.5092896174865</v>
       </c>
       <c r="I43" s="23"/>
       <c r="J43" s="23"/>
@@ -3287,25 +3287,25 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C44" s="23" t="s">
         <v>39</v>
       </c>
       <c r="D44" s="24"/>
       <c r="E44" s="24">
-        <v>2145697</v>
+        <v>2190061</v>
       </c>
       <c r="F44" s="24"/>
       <c r="G44" s="26">
-        <v>64899</v>
+        <v>32112</v>
       </c>
       <c r="H44" s="25">
         <f t="shared" si="1"/>
-        <v>33.062096488389649</v>
+        <v>68.200703786746388</v>
       </c>
       <c r="I44" s="23"/>
       <c r="J44" s="23"/>
@@ -3325,22 +3325,22 @@
         <v>41</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C45" s="23" t="s">
         <v>35</v>
       </c>
       <c r="D45" s="24"/>
       <c r="E45" s="24">
-        <v>695213</v>
+        <v>2145697</v>
       </c>
       <c r="F45" s="24"/>
       <c r="G45" s="26">
-        <v>368</v>
+        <v>187887</v>
       </c>
       <c r="H45" s="25">
         <f t="shared" si="1"/>
-        <v>1889.1657608695652</v>
+        <v>11.420146151676274</v>
       </c>
       <c r="I45" s="23"/>
       <c r="J45" s="23"/>
@@ -3360,22 +3360,22 @@
         <v>41</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C46" s="23" t="s">
         <v>21</v>
       </c>
       <c r="D46" s="24"/>
       <c r="E46" s="24">
-        <v>695213</v>
+        <v>2145697</v>
       </c>
       <c r="F46" s="24"/>
       <c r="G46" s="26">
-        <v>79</v>
+        <v>1615</v>
       </c>
       <c r="H46" s="25">
         <f t="shared" si="1"/>
-        <v>8800.164556962025</v>
+        <v>1328.6049535603715</v>
       </c>
       <c r="I46" s="23"/>
       <c r="J46" s="23"/>
@@ -3395,22 +3395,22 @@
         <v>41</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C47" s="23" t="s">
         <v>39</v>
       </c>
       <c r="D47" s="24"/>
       <c r="E47" s="24">
-        <v>695213</v>
+        <v>2145697</v>
       </c>
       <c r="F47" s="24"/>
       <c r="G47" s="26">
-        <v>2638</v>
+        <v>64899</v>
       </c>
       <c r="H47" s="25">
         <f t="shared" si="1"/>
-        <v>263.53790750568612</v>
+        <v>33.062096488389649</v>
       </c>
       <c r="I47" s="23"/>
       <c r="J47" s="23"/>
@@ -3430,22 +3430,22 @@
         <v>41</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C48" s="23" t="s">
         <v>35</v>
       </c>
       <c r="D48" s="24"/>
       <c r="E48" s="24">
-        <v>4856625</v>
+        <v>695213</v>
       </c>
       <c r="F48" s="24"/>
       <c r="G48" s="26">
-        <v>799443</v>
+        <v>368</v>
       </c>
       <c r="H48" s="25">
         <f t="shared" si="1"/>
-        <v>6.0750109763923135</v>
+        <v>1889.1657608695652</v>
       </c>
       <c r="I48" s="23"/>
       <c r="J48" s="23"/>
@@ -3465,22 +3465,22 @@
         <v>41</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C49" s="23" t="s">
         <v>21</v>
       </c>
       <c r="D49" s="24"/>
       <c r="E49" s="24">
-        <v>4856625</v>
+        <v>695213</v>
       </c>
       <c r="F49" s="24"/>
       <c r="G49" s="26">
-        <v>11563</v>
+        <v>79</v>
       </c>
       <c r="H49" s="25">
         <f t="shared" si="1"/>
-        <v>420.01426965320417</v>
+        <v>8800.164556962025</v>
       </c>
       <c r="I49" s="23"/>
       <c r="J49" s="23"/>
@@ -3500,22 +3500,22 @@
         <v>41</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C50" s="23" t="s">
         <v>39</v>
       </c>
       <c r="D50" s="24"/>
       <c r="E50" s="24">
-        <v>4856625</v>
+        <v>695213</v>
       </c>
       <c r="F50" s="24"/>
       <c r="G50" s="26">
-        <v>390548</v>
+        <v>2638</v>
       </c>
       <c r="H50" s="25">
         <f t="shared" si="1"/>
-        <v>12.435411268269201</v>
+        <v>263.53790750568612</v>
       </c>
       <c r="I50" s="23"/>
       <c r="J50" s="23"/>
@@ -3532,128 +3532,107 @@
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D51" s="24">
-        <v>4791000000</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D51" s="24"/>
       <c r="E51" s="24">
-        <f>D51/10</f>
-        <v>479100000</v>
+        <v>4856625</v>
       </c>
       <c r="F51" s="24"/>
       <c r="G51" s="26">
-        <v>2800000</v>
+        <v>799443</v>
       </c>
       <c r="H51" s="25">
         <f t="shared" si="1"/>
-        <v>171.10714285714286</v>
-      </c>
-      <c r="I51" s="23">
-        <v>2018</v>
-      </c>
-      <c r="J51" s="23">
-        <v>2027</v>
-      </c>
+        <v>6.0750109763923135</v>
+      </c>
+      <c r="I51" s="23"/>
+      <c r="J51" s="23"/>
       <c r="K51" s="23">
-        <v>2017</v>
+        <v>2002</v>
       </c>
       <c r="L51" s="23" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="M51" s="23"/>
       <c r="N51" s="23" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="23" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D52" s="24">
-        <v>4791000000</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D52" s="24"/>
       <c r="E52" s="24">
-        <f>D52/10</f>
-        <v>479100000</v>
+        <v>4856625</v>
       </c>
       <c r="F52" s="24"/>
       <c r="G52" s="26">
-        <v>2900000</v>
+        <v>11563</v>
       </c>
       <c r="H52" s="25">
         <f t="shared" si="1"/>
-        <v>165.20689655172413</v>
-      </c>
-      <c r="I52" s="23">
-        <v>2018</v>
-      </c>
-      <c r="J52" s="23">
-        <v>2027</v>
-      </c>
+        <v>420.01426965320417</v>
+      </c>
+      <c r="I52" s="23"/>
+      <c r="J52" s="23"/>
       <c r="K52" s="23">
-        <v>2017</v>
+        <v>2002</v>
       </c>
       <c r="L52" s="23" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="M52" s="23"/>
       <c r="N52" s="23" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D53" s="24">
-        <v>4791000000</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D53" s="24"/>
       <c r="E53" s="24">
-        <f>D53/10</f>
-        <v>479100000</v>
+        <v>4856625</v>
       </c>
       <c r="F53" s="24"/>
       <c r="G53" s="26">
-        <v>40000</v>
+        <v>390548</v>
       </c>
       <c r="H53" s="25">
         <f t="shared" si="1"/>
-        <v>11977.5</v>
-      </c>
-      <c r="I53" s="23">
-        <v>2018</v>
-      </c>
-      <c r="J53" s="23">
-        <v>2027</v>
-      </c>
+        <v>12.435411268269201</v>
+      </c>
+      <c r="I53" s="23"/>
+      <c r="J53" s="23"/>
       <c r="K53" s="23">
-        <v>2017</v>
+        <v>2002</v>
       </c>
       <c r="L53" s="23" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="M53" s="23"/>
       <c r="N53" s="23" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
@@ -3664,33 +3643,38 @@
         <v>42</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D54" s="24"/>
+        <v>22</v>
+      </c>
+      <c r="D54" s="24">
+        <v>4791000000</v>
+      </c>
       <c r="E54" s="24">
-        <v>240000000</v>
+        <f>D54/10</f>
+        <v>479100000</v>
       </c>
       <c r="F54" s="24"/>
-      <c r="G54" s="24">
-        <v>34800</v>
+      <c r="G54" s="26">
+        <v>2800000</v>
       </c>
       <c r="H54" s="25">
         <f t="shared" si="1"/>
-        <v>6896.5517241379312</v>
-      </c>
-      <c r="I54" s="23"/>
-      <c r="J54" s="23"/>
+        <v>171.10714285714286</v>
+      </c>
+      <c r="I54" s="23">
+        <v>2018</v>
+      </c>
+      <c r="J54" s="23">
+        <v>2027</v>
+      </c>
       <c r="K54" s="23">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="L54" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="M54" s="23" t="s">
-        <v>51</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="M54" s="23"/>
       <c r="N54" s="23" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
@@ -3701,33 +3685,38 @@
         <v>42</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D55" s="24"/>
+        <v>44</v>
+      </c>
+      <c r="D55" s="24">
+        <v>4791000000</v>
+      </c>
       <c r="E55" s="24">
-        <v>240000000</v>
+        <f>D55/10</f>
+        <v>479100000</v>
       </c>
       <c r="F55" s="24"/>
-      <c r="G55" s="24">
-        <v>48700000</v>
+      <c r="G55" s="26">
+        <v>2900000</v>
       </c>
       <c r="H55" s="25">
         <f t="shared" si="1"/>
-        <v>4.9281314168377826</v>
-      </c>
-      <c r="I55" s="23"/>
-      <c r="J55" s="23"/>
+        <v>165.20689655172413</v>
+      </c>
+      <c r="I55" s="23">
+        <v>2018</v>
+      </c>
+      <c r="J55" s="23">
+        <v>2027</v>
+      </c>
       <c r="K55" s="23">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="L55" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="M55" s="23" t="s">
-        <v>51</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="M55" s="23"/>
       <c r="N55" s="23" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
@@ -3738,33 +3727,38 @@
         <v>42</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D56" s="24"/>
+        <v>45</v>
+      </c>
+      <c r="D56" s="24">
+        <v>4791000000</v>
+      </c>
       <c r="E56" s="24">
-        <v>240000000</v>
+        <f>D56/10</f>
+        <v>479100000</v>
       </c>
       <c r="F56" s="24"/>
-      <c r="G56" s="24">
-        <f>E56/H56</f>
-        <v>1666666.6666666667</v>
+      <c r="G56" s="26">
+        <v>40000</v>
       </c>
       <c r="H56" s="25">
-        <v>144</v>
-      </c>
-      <c r="I56" s="23"/>
-      <c r="J56" s="23"/>
+        <f t="shared" si="1"/>
+        <v>11977.5</v>
+      </c>
+      <c r="I56" s="23">
+        <v>2018</v>
+      </c>
+      <c r="J56" s="23">
+        <v>2027</v>
+      </c>
       <c r="K56" s="23">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="L56" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="M56" s="23" t="s">
-        <v>51</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="M56" s="23"/>
       <c r="N56" s="23" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
@@ -3775,19 +3769,19 @@
         <v>42</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D57" s="24"/>
       <c r="E57" s="24">
-        <v>328000000</v>
+        <v>240000000</v>
       </c>
       <c r="F57" s="24"/>
       <c r="G57" s="24">
-        <v>13900000</v>
+        <v>34800</v>
       </c>
       <c r="H57" s="25">
-        <f>E57/G57</f>
-        <v>23.597122302158272</v>
+        <f t="shared" si="1"/>
+        <v>6896.5517241379312</v>
       </c>
       <c r="I57" s="23"/>
       <c r="J57" s="23"/>
@@ -3798,7 +3792,7 @@
         <v>31</v>
       </c>
       <c r="M57" s="23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="N57" s="23" t="s">
         <v>52</v>
@@ -3812,19 +3806,19 @@
         <v>42</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D58" s="24"/>
       <c r="E58" s="24">
-        <v>328000000</v>
+        <v>240000000</v>
       </c>
       <c r="F58" s="24"/>
       <c r="G58" s="24">
-        <f>E58/H58</f>
-        <v>2582677.1653543306</v>
+        <v>48700000</v>
       </c>
       <c r="H58" s="25">
-        <v>127</v>
+        <f t="shared" si="1"/>
+        <v>4.9281314168377826</v>
       </c>
       <c r="I58" s="23"/>
       <c r="J58" s="23"/>
@@ -3835,7 +3829,7 @@
         <v>31</v>
       </c>
       <c r="M58" s="23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="N58" s="23" t="s">
         <v>52</v>
@@ -3843,440 +3837,408 @@
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="23" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B59" s="23" t="s">
         <v>42</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D59" s="24"/>
       <c r="E59" s="24">
-        <v>18747118</v>
+        <v>240000000</v>
       </c>
       <c r="F59" s="24"/>
       <c r="G59" s="24">
-        <v>52525</v>
+        <f>E59/H59</f>
+        <v>1666666.6666666667</v>
       </c>
       <c r="H59" s="25">
-        <f t="shared" ref="H59:H84" si="2">E59/G59</f>
-        <v>356.91800095192764</v>
-      </c>
-      <c r="I59" s="23">
-        <v>2022</v>
-      </c>
-      <c r="J59" s="23">
-        <v>2032</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="I59" s="23"/>
+      <c r="J59" s="23"/>
       <c r="K59" s="23">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="L59" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="M59" s="23"/>
+        <v>31</v>
+      </c>
+      <c r="M59" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="N59" s="23" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="23" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B60" s="23" t="s">
         <v>42</v>
       </c>
       <c r="C60" s="23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D60" s="24"/>
       <c r="E60" s="24">
+        <v>328000000</v>
+      </c>
+      <c r="F60" s="24"/>
+      <c r="G60" s="24">
+        <v>13900000</v>
+      </c>
+      <c r="H60" s="25">
+        <f>E60/G60</f>
+        <v>23.597122302158272</v>
+      </c>
+      <c r="I60" s="23"/>
+      <c r="J60" s="23"/>
+      <c r="K60" s="23">
+        <v>2014</v>
+      </c>
+      <c r="L60" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="M60" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="N60" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A61" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24">
+        <v>328000000</v>
+      </c>
+      <c r="F61" s="24"/>
+      <c r="G61" s="24">
+        <f>E61/H61</f>
+        <v>2582677.1653543306</v>
+      </c>
+      <c r="H61" s="25">
+        <v>127</v>
+      </c>
+      <c r="I61" s="23"/>
+      <c r="J61" s="23"/>
+      <c r="K61" s="23">
+        <v>2014</v>
+      </c>
+      <c r="L61" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="M61" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="N61" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A62" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C62" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24">
         <v>18747118</v>
       </c>
-      <c r="F60" s="24"/>
-      <c r="G60" s="27">
+      <c r="F62" s="24"/>
+      <c r="G62" s="24">
+        <v>52525</v>
+      </c>
+      <c r="H62" s="25">
+        <f t="shared" ref="H62:H87" si="2">E62/G62</f>
+        <v>356.91800095192764</v>
+      </c>
+      <c r="I62" s="23">
+        <v>2022</v>
+      </c>
+      <c r="J62" s="23">
+        <v>2032</v>
+      </c>
+      <c r="K62" s="23">
+        <v>2016</v>
+      </c>
+      <c r="L62" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="M62" s="23"/>
+      <c r="N62" s="23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A63" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C63" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24">
+        <v>18747118</v>
+      </c>
+      <c r="F63" s="24"/>
+      <c r="G63" s="27">
         <v>1302.6363636363601</v>
       </c>
-      <c r="H60" s="25">
+      <c r="H63" s="25">
         <f t="shared" si="2"/>
         <v>14391.67408751487</v>
       </c>
-      <c r="I60" s="23">
+      <c r="I63" s="23">
         <v>2022</v>
       </c>
-      <c r="J60" s="23">
+      <c r="J63" s="23">
         <v>2032</v>
       </c>
-      <c r="K60" s="23">
+      <c r="K63" s="23">
         <v>2016</v>
       </c>
-      <c r="L60" s="23" t="s">
+      <c r="L63" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="M60" s="23"/>
-      <c r="N60" s="23" t="s">
+      <c r="M63" s="23"/>
+      <c r="N63" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="S60" s="4"/>
-      <c r="U60" s="22"/>
-    </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A61" s="23" t="s">
+      <c r="S63" s="4"/>
+      <c r="U63" s="22"/>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A64" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B61" s="23" t="s">
+      <c r="B64" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C61" s="23" t="s">
+      <c r="C64" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D61" s="24"/>
-      <c r="E61" s="24">
+      <c r="D64" s="24"/>
+      <c r="E64" s="24">
         <v>18747118</v>
       </c>
-      <c r="F61" s="24"/>
-      <c r="G61" s="27">
+      <c r="F64" s="24"/>
+      <c r="G64" s="27">
         <v>9228.4545454545496</v>
       </c>
-      <c r="H61" s="25">
+      <c r="H64" s="25">
         <f t="shared" si="2"/>
         <v>2031.4471841044981</v>
       </c>
-      <c r="I61" s="23">
+      <c r="I64" s="23">
         <v>2022</v>
       </c>
-      <c r="J61" s="23">
+      <c r="J64" s="23">
         <v>2032</v>
       </c>
-      <c r="K61" s="23">
+      <c r="K64" s="23">
         <v>2016</v>
       </c>
-      <c r="L61" s="23" t="s">
+      <c r="L64" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="M61" s="23"/>
-      <c r="N61" s="23" t="s">
+      <c r="M64" s="23"/>
+      <c r="N64" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="S61" s="4"/>
-      <c r="T61" s="22"/>
-      <c r="U61" s="22"/>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A62" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B62" s="23" t="s">
+      <c r="S64" s="4"/>
+      <c r="T64" s="22"/>
+      <c r="U64" s="22"/>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A65" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C62" s="23" t="s">
+      <c r="C65" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D62" s="24">
+      <c r="D65" s="24">
         <v>64090055</v>
       </c>
-      <c r="E62" s="24">
-        <f t="shared" ref="E62:E109" si="3">D62/10</f>
+      <c r="E65" s="24">
+        <f t="shared" ref="E65:E112" si="3">D65/10</f>
         <v>6409005.5</v>
       </c>
-      <c r="F62" s="24">
+      <c r="F65" s="24">
         <v>1775985</v>
       </c>
-      <c r="G62" s="24">
-        <f t="shared" ref="G62:G85" si="4">F62/10</f>
+      <c r="G65" s="24">
+        <f t="shared" ref="G65:G88" si="4">F65/10</f>
         <v>177598.5</v>
       </c>
-      <c r="H62" s="25">
+      <c r="H65" s="25">
         <f t="shared" si="2"/>
         <v>36.087047469432456</v>
       </c>
-      <c r="I62" s="23">
+      <c r="I65" s="23">
         <v>2018</v>
       </c>
-      <c r="J62" s="23">
+      <c r="J65" s="23">
         <v>2027</v>
       </c>
-      <c r="K62" s="23">
+      <c r="K65" s="23">
         <v>2015</v>
       </c>
-      <c r="L62" s="23" t="s">
+      <c r="L65" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="M62" s="23" t="s">
+      <c r="M65" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="N62" s="23" t="s">
+      <c r="N65" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="S62" s="4"/>
-      <c r="T62" s="22"/>
-      <c r="U62" s="22"/>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A63" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B63" s="23" t="s">
+      <c r="S65" s="4"/>
+      <c r="T65" s="22"/>
+      <c r="U65" s="22"/>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A66" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C63" s="23" t="s">
+      <c r="C66" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D63" s="24">
+      <c r="D66" s="24">
         <v>64090055</v>
       </c>
-      <c r="E63" s="24">
+      <c r="E66" s="24">
         <f t="shared" si="3"/>
         <v>6409005.5</v>
       </c>
-      <c r="F63" s="24">
+      <c r="F66" s="24">
         <v>6344</v>
       </c>
-      <c r="G63" s="24">
+      <c r="G66" s="24">
         <f t="shared" si="4"/>
         <v>634.4</v>
       </c>
-      <c r="H63" s="25">
+      <c r="H66" s="25">
         <f t="shared" si="2"/>
         <v>10102.467686002523</v>
       </c>
-      <c r="I63" s="23">
+      <c r="I66" s="23">
         <v>2018</v>
       </c>
-      <c r="J63" s="23">
+      <c r="J66" s="23">
         <v>2027</v>
       </c>
-      <c r="K63" s="23">
+      <c r="K66" s="23">
         <v>2015</v>
       </c>
-      <c r="L63" s="23" t="s">
+      <c r="L66" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="M63" s="23" t="s">
+      <c r="M66" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="N63" s="23" t="s">
+      <c r="N66" s="23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A64" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B64" s="23" t="s">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A67" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C64" s="23" t="s">
+      <c r="C67" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D64" s="24">
+      <c r="D67" s="24">
         <v>64090055</v>
       </c>
-      <c r="E64" s="24">
+      <c r="E67" s="24">
         <f t="shared" si="3"/>
         <v>6409005.5</v>
       </c>
-      <c r="F64" s="24">
+      <c r="F67" s="24">
         <v>6160965</v>
       </c>
-      <c r="G64" s="24">
+      <c r="G67" s="24">
         <f t="shared" si="4"/>
         <v>616096.5</v>
       </c>
-      <c r="H64" s="25">
+      <c r="H67" s="25">
         <f t="shared" si="2"/>
         <v>10.402600079695308</v>
       </c>
-      <c r="I64" s="23">
+      <c r="I67" s="23">
         <v>2018</v>
       </c>
-      <c r="J64" s="23">
+      <c r="J67" s="23">
         <v>2027</v>
       </c>
-      <c r="K64" s="23">
+      <c r="K67" s="23">
         <v>2015</v>
       </c>
-      <c r="L64" s="23" t="s">
+      <c r="L67" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="M64" s="23" t="s">
+      <c r="M67" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="N64" s="23" t="s">
+      <c r="N67" s="23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A65" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B65" s="23" t="s">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A68" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C65" s="23" t="s">
+      <c r="C68" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="24">
+      <c r="D68" s="24">
         <v>64090055</v>
       </c>
-      <c r="E65" s="24">
+      <c r="E68" s="24">
         <f t="shared" si="3"/>
         <v>6409005.5</v>
       </c>
-      <c r="F65" s="24">
+      <c r="F68" s="24">
         <v>333802.36979166669</v>
       </c>
-      <c r="G65" s="24">
+      <c r="G68" s="24">
         <f t="shared" si="4"/>
         <v>33380.236979166672</v>
       </c>
-      <c r="H65" s="25">
+      <c r="H68" s="25">
         <f t="shared" si="2"/>
         <v>191.99999999999997</v>
-      </c>
-      <c r="I65" s="23">
-        <v>2018</v>
-      </c>
-      <c r="J65" s="23">
-        <v>2027</v>
-      </c>
-      <c r="K65" s="23">
-        <v>2015</v>
-      </c>
-      <c r="L65" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="M65" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="N65" s="23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A66" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B66" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C66" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="D66" s="24">
-        <v>117831196</v>
-      </c>
-      <c r="E66" s="24">
-        <f t="shared" si="3"/>
-        <v>11783119.6</v>
-      </c>
-      <c r="F66" s="26">
-        <v>3225501</v>
-      </c>
-      <c r="G66" s="24">
-        <f t="shared" si="4"/>
-        <v>322550.09999999998</v>
-      </c>
-      <c r="H66" s="25">
-        <f t="shared" si="2"/>
-        <v>36.531129892689542</v>
-      </c>
-      <c r="I66" s="23">
-        <v>2018</v>
-      </c>
-      <c r="J66" s="23">
-        <v>2027</v>
-      </c>
-      <c r="K66" s="23">
-        <v>2015</v>
-      </c>
-      <c r="L66" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="M66" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="N66" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="S66" s="4"/>
-    </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A67" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B67" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C67" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D67" s="24">
-        <v>117831196</v>
-      </c>
-      <c r="E67" s="24">
-        <f t="shared" si="3"/>
-        <v>11783119.6</v>
-      </c>
-      <c r="F67" s="26">
-        <v>8877</v>
-      </c>
-      <c r="G67" s="24">
-        <f t="shared" si="4"/>
-        <v>887.7</v>
-      </c>
-      <c r="H67" s="25">
-        <f t="shared" si="2"/>
-        <v>13273.763208291088</v>
-      </c>
-      <c r="I67" s="23">
-        <v>2018</v>
-      </c>
-      <c r="J67" s="23">
-        <v>2027</v>
-      </c>
-      <c r="K67" s="23">
-        <v>2015</v>
-      </c>
-      <c r="L67" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="M67" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="N67" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="S67" s="4"/>
-    </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A68" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B68" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C68" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="D68" s="24">
-        <v>117831196</v>
-      </c>
-      <c r="E68" s="24">
-        <f t="shared" si="3"/>
-        <v>11783119.6</v>
-      </c>
-      <c r="F68" s="26">
-        <v>8233918</v>
-      </c>
-      <c r="G68" s="24">
-        <f t="shared" si="4"/>
-        <v>823391.8</v>
-      </c>
-      <c r="H68" s="25">
-        <f t="shared" si="2"/>
-        <v>14.310465078714651</v>
       </c>
       <c r="I68" s="23">
         <v>2018</v>
@@ -4305,7 +4267,7 @@
         <v>56</v>
       </c>
       <c r="C69" s="23" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D69" s="24">
         <v>117831196</v>
@@ -4314,16 +4276,16 @@
         <f t="shared" si="3"/>
         <v>11783119.6</v>
       </c>
-      <c r="F69" s="24">
-        <v>416364.65017667843</v>
+      <c r="F69" s="26">
+        <v>3225501</v>
       </c>
       <c r="G69" s="24">
         <f t="shared" si="4"/>
-        <v>41636.465017667841</v>
+        <v>322550.09999999998</v>
       </c>
       <c r="H69" s="25">
         <f t="shared" si="2"/>
-        <v>283</v>
+        <v>36.531129892689542</v>
       </c>
       <c r="I69" s="23">
         <v>2018</v>
@@ -4343,34 +4305,35 @@
       <c r="N69" s="23" t="s">
         <v>59</v>
       </c>
+      <c r="S69" s="4"/>
     </row>
     <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" s="23" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B70" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C70" s="23" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D70" s="24">
-        <v>1761981734</v>
+        <v>117831196</v>
       </c>
       <c r="E70" s="24">
         <f t="shared" si="3"/>
-        <v>176198173.40000001</v>
-      </c>
-      <c r="F70" s="24">
-        <v>46083379</v>
+        <v>11783119.6</v>
+      </c>
+      <c r="F70" s="26">
+        <v>8877</v>
       </c>
       <c r="G70" s="24">
         <f t="shared" si="4"/>
-        <v>4608337.9000000004</v>
+        <v>887.7</v>
       </c>
       <c r="H70" s="25">
         <f t="shared" si="2"/>
-        <v>38.234647116479891</v>
+        <v>13273.763208291088</v>
       </c>
       <c r="I70" s="23">
         <v>2018</v>
@@ -4390,34 +4353,35 @@
       <c r="N70" s="23" t="s">
         <v>59</v>
       </c>
+      <c r="S70" s="4"/>
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" s="23" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B71" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C71" s="23" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D71" s="24">
-        <v>1761981734</v>
+        <v>117831196</v>
       </c>
       <c r="E71" s="24">
         <f t="shared" si="3"/>
-        <v>176198173.40000001</v>
-      </c>
-      <c r="F71" s="24">
-        <v>106007</v>
+        <v>11783119.6</v>
+      </c>
+      <c r="F71" s="26">
+        <v>8233918</v>
       </c>
       <c r="G71" s="24">
         <f t="shared" si="4"/>
-        <v>10600.7</v>
+        <v>823391.8</v>
       </c>
       <c r="H71" s="25">
         <f t="shared" si="2"/>
-        <v>16621.371550935313</v>
+        <v>14.310465078714651</v>
       </c>
       <c r="I71" s="23">
         <v>2018</v>
@@ -4437,35 +4401,34 @@
       <c r="N71" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="W71" s="4"/>
     </row>
     <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" s="23" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B72" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C72" s="23" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="D72" s="24">
-        <v>1761981734</v>
+        <v>117831196</v>
       </c>
       <c r="E72" s="24">
         <f t="shared" si="3"/>
-        <v>176198173.40000001</v>
+        <v>11783119.6</v>
       </c>
       <c r="F72" s="24">
-        <v>117772708</v>
+        <v>416364.65017667843</v>
       </c>
       <c r="G72" s="24">
         <f t="shared" si="4"/>
-        <v>11777270.800000001</v>
+        <v>41636.465017667841</v>
       </c>
       <c r="H72" s="25">
         <f t="shared" si="2"/>
-        <v>14.960866264533884</v>
+        <v>283</v>
       </c>
       <c r="I72" s="23">
         <v>2018</v>
@@ -4494,7 +4457,7 @@
         <v>56</v>
       </c>
       <c r="C73" s="23" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D73" s="24">
         <v>1761981734</v>
@@ -4504,15 +4467,15 @@
         <v>176198173.40000001</v>
       </c>
       <c r="F73" s="24">
-        <v>2996567.5748299318</v>
+        <v>46083379</v>
       </c>
       <c r="G73" s="24">
         <f t="shared" si="4"/>
-        <v>299656.75748299318</v>
+        <v>4608337.9000000004</v>
       </c>
       <c r="H73" s="25">
         <f t="shared" si="2"/>
-        <v>588</v>
+        <v>38.234647116479891</v>
       </c>
       <c r="I73" s="23">
         <v>2018</v>
@@ -4535,31 +4498,31 @@
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" s="23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B74" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C74" s="23" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D74" s="24">
-        <v>342230664</v>
+        <v>1761981734</v>
       </c>
       <c r="E74" s="24">
         <f t="shared" si="3"/>
-        <v>34223066.399999999</v>
+        <v>176198173.40000001</v>
       </c>
       <c r="F74" s="24">
-        <v>10650771</v>
+        <v>106007</v>
       </c>
       <c r="G74" s="24">
         <f t="shared" si="4"/>
-        <v>1065077.1000000001</v>
+        <v>10600.7</v>
       </c>
       <c r="H74" s="25">
         <f t="shared" si="2"/>
-        <v>32.132008471499383</v>
+        <v>16621.371550935313</v>
       </c>
       <c r="I74" s="23">
         <v>2018</v>
@@ -4579,34 +4542,35 @@
       <c r="N74" s="23" t="s">
         <v>59</v>
       </c>
+      <c r="W74" s="4"/>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" s="23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B75" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C75" s="23" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D75" s="24">
-        <v>342230664</v>
+        <v>1761981734</v>
       </c>
       <c r="E75" s="24">
         <f t="shared" si="3"/>
-        <v>34223066.399999999</v>
+        <v>176198173.40000001</v>
       </c>
       <c r="F75" s="24">
-        <v>91934</v>
+        <v>117772708</v>
       </c>
       <c r="G75" s="24">
         <f t="shared" si="4"/>
-        <v>9193.4</v>
+        <v>11777270.800000001</v>
       </c>
       <c r="H75" s="25">
         <f t="shared" si="2"/>
-        <v>3722.5690604129049</v>
+        <v>14.960866264533884</v>
       </c>
       <c r="I75" s="23">
         <v>2018</v>
@@ -4629,31 +4593,31 @@
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" s="23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B76" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C76" s="23" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="D76" s="24">
-        <v>342230664</v>
+        <v>1761981734</v>
       </c>
       <c r="E76" s="24">
         <f t="shared" si="3"/>
-        <v>34223066.399999999</v>
+        <v>176198173.40000001</v>
       </c>
       <c r="F76" s="24">
-        <v>28485738</v>
+        <v>2996567.5748299318</v>
       </c>
       <c r="G76" s="24">
         <f t="shared" si="4"/>
-        <v>2848573.8</v>
+        <v>299656.75748299318</v>
       </c>
       <c r="H76" s="25">
         <f t="shared" si="2"/>
-        <v>12.014105585047508</v>
+        <v>588</v>
       </c>
       <c r="I76" s="23">
         <v>2018</v>
@@ -4682,7 +4646,7 @@
         <v>56</v>
       </c>
       <c r="C77" s="23" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D77" s="24">
         <v>342230664</v>
@@ -4692,15 +4656,15 @@
         <v>34223066.399999999</v>
       </c>
       <c r="F77" s="24">
-        <v>2950264.3448275863</v>
+        <v>10650771</v>
       </c>
       <c r="G77" s="24">
         <f t="shared" si="4"/>
-        <v>295026.43448275863</v>
+        <v>1065077.1000000001</v>
       </c>
       <c r="H77" s="25">
         <f t="shared" si="2"/>
-        <v>115.99999999999999</v>
+        <v>32.132008471499383</v>
       </c>
       <c r="I77" s="23">
         <v>2018</v>
@@ -4723,31 +4687,31 @@
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" s="23" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B78" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C78" s="23" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D78" s="24">
-        <v>77669464</v>
+        <v>342230664</v>
       </c>
       <c r="E78" s="24">
         <f t="shared" si="3"/>
-        <v>7766946.4000000004</v>
+        <v>34223066.399999999</v>
       </c>
       <c r="F78" s="24">
-        <v>2242237</v>
+        <v>91934</v>
       </c>
       <c r="G78" s="24">
         <f t="shared" si="4"/>
-        <v>224223.7</v>
+        <v>9193.4</v>
       </c>
       <c r="H78" s="25">
         <f t="shared" si="2"/>
-        <v>34.639274974054928</v>
+        <v>3722.5690604129049</v>
       </c>
       <c r="I78" s="23">
         <v>2018</v>
@@ -4770,31 +4734,31 @@
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" s="23" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B79" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C79" s="23" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D79" s="24">
-        <v>77669464</v>
+        <v>342230664</v>
       </c>
       <c r="E79" s="24">
         <f t="shared" si="3"/>
-        <v>7766946.4000000004</v>
+        <v>34223066.399999999</v>
       </c>
       <c r="F79" s="24">
-        <v>30528</v>
+        <v>28485738</v>
       </c>
       <c r="G79" s="24">
         <f t="shared" si="4"/>
-        <v>3052.8</v>
+        <v>2848573.8</v>
       </c>
       <c r="H79" s="25">
         <f t="shared" si="2"/>
-        <v>2544.204140461216</v>
+        <v>12.014105585047508</v>
       </c>
       <c r="I79" s="23">
         <v>2018</v>
@@ -4817,31 +4781,31 @@
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" s="23" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B80" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C80" s="23" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="D80" s="24">
-        <v>77669464</v>
+        <v>342230664</v>
       </c>
       <c r="E80" s="24">
         <f t="shared" si="3"/>
-        <v>7766946.4000000004</v>
+        <v>34223066.399999999</v>
       </c>
       <c r="F80" s="24">
-        <v>21333511</v>
+        <v>2950264.3448275863</v>
       </c>
       <c r="G80" s="24">
         <f t="shared" si="4"/>
-        <v>2133351.1</v>
+        <v>295026.43448275863</v>
       </c>
       <c r="H80" s="25">
         <f t="shared" si="2"/>
-        <v>3.6407258045804087</v>
+        <v>115.99999999999999</v>
       </c>
       <c r="I80" s="23">
         <v>2018</v>
@@ -4870,7 +4834,7 @@
         <v>56</v>
       </c>
       <c r="C81" s="23" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D81" s="24">
         <v>77669464</v>
@@ -4880,15 +4844,15 @@
         <v>7766946.4000000004</v>
       </c>
       <c r="F81" s="24">
-        <v>1049587.3513513512</v>
+        <v>2242237</v>
       </c>
       <c r="G81" s="24">
         <f t="shared" si="4"/>
-        <v>104958.73513513512</v>
+        <v>224223.7</v>
       </c>
       <c r="H81" s="25">
         <f t="shared" si="2"/>
-        <v>74.000000000000014</v>
+        <v>34.639274974054928</v>
       </c>
       <c r="I81" s="23">
         <v>2018</v>
@@ -4911,31 +4875,31 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="23" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B82" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C82" s="23" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D82" s="24">
-        <v>36891487</v>
+        <v>77669464</v>
       </c>
       <c r="E82" s="24">
         <f t="shared" si="3"/>
-        <v>3689148.7</v>
+        <v>7766946.4000000004</v>
       </c>
       <c r="F82" s="24">
-        <v>1078428</v>
+        <v>30528</v>
       </c>
       <c r="G82" s="24">
         <f t="shared" si="4"/>
-        <v>107842.8</v>
+        <v>3052.8</v>
       </c>
       <c r="H82" s="25">
         <f t="shared" si="2"/>
-        <v>34.208576743185453</v>
+        <v>2544.204140461216</v>
       </c>
       <c r="I82" s="23">
         <v>2018</v>
@@ -4949,7 +4913,7 @@
       <c r="L82" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="M82" s="28" t="s">
+      <c r="M82" s="23" t="s">
         <v>93</v>
       </c>
       <c r="N82" s="23" t="s">
@@ -4958,31 +4922,31 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="23" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B83" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C83" s="23" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D83" s="24">
-        <v>36891487</v>
+        <v>77669464</v>
       </c>
       <c r="E83" s="24">
         <f t="shared" si="3"/>
-        <v>3689148.7</v>
+        <v>7766946.4000000004</v>
       </c>
       <c r="F83" s="24">
-        <v>3025</v>
+        <v>21333511</v>
       </c>
       <c r="G83" s="24">
         <f t="shared" si="4"/>
-        <v>302.5</v>
+        <v>2133351.1</v>
       </c>
       <c r="H83" s="25">
         <f t="shared" si="2"/>
-        <v>12195.532892561983</v>
+        <v>3.6407258045804087</v>
       </c>
       <c r="I83" s="23">
         <v>2018</v>
@@ -4996,7 +4960,7 @@
       <c r="L83" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="M83" s="28" t="s">
+      <c r="M83" s="23" t="s">
         <v>93</v>
       </c>
       <c r="N83" s="23" t="s">
@@ -5005,31 +4969,31 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="23" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B84" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C84" s="23" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="D84" s="24">
-        <v>36891487</v>
+        <v>77669464</v>
       </c>
       <c r="E84" s="24">
         <f t="shared" si="3"/>
-        <v>3689148.7</v>
+        <v>7766946.4000000004</v>
       </c>
       <c r="F84" s="24">
-        <v>3505164</v>
+        <v>1049587.3513513512</v>
       </c>
       <c r="G84" s="24">
         <f t="shared" si="4"/>
-        <v>350516.4</v>
+        <v>104958.73513513512</v>
       </c>
       <c r="H84" s="25">
         <f t="shared" si="2"/>
-        <v>10.524896124689173</v>
+        <v>74.000000000000014</v>
       </c>
       <c r="I84" s="23">
         <v>2018</v>
@@ -5043,7 +5007,7 @@
       <c r="L84" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="M84" s="28" t="s">
+      <c r="M84" s="23" t="s">
         <v>93</v>
       </c>
       <c r="N84" s="23" t="s">
@@ -5058,7 +5022,7 @@
         <v>56</v>
       </c>
       <c r="C85" s="23" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D85" s="24">
         <v>36891487</v>
@@ -5068,14 +5032,15 @@
         <v>3689148.7</v>
       </c>
       <c r="F85" s="24">
-        <v>275309.60447761195</v>
+        <v>1078428</v>
       </c>
       <c r="G85" s="24">
         <f t="shared" si="4"/>
-        <v>27530.960447761194</v>
+        <v>107842.8</v>
       </c>
       <c r="H85" s="25">
-        <v>134</v>
+        <f t="shared" si="2"/>
+        <v>34.208576743185453</v>
       </c>
       <c r="I85" s="23">
         <v>2018</v>
@@ -5098,30 +5063,31 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="23" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B86" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C86" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="D86" s="29">
-        <v>37213746</v>
+        <v>49</v>
+      </c>
+      <c r="D86" s="24">
+        <v>36891487</v>
       </c>
       <c r="E86" s="24">
         <f t="shared" si="3"/>
-        <v>3721374.6</v>
+        <v>3689148.7</v>
       </c>
       <c r="F86" s="24">
-        <v>1775985</v>
+        <v>3025</v>
       </c>
       <c r="G86" s="24">
-        <v>177598.5</v>
+        <f t="shared" si="4"/>
+        <v>302.5</v>
       </c>
       <c r="H86" s="25">
-        <f t="shared" ref="H86:H109" si="5">E86/G86</f>
-        <v>20.95386278600326</v>
+        <f t="shared" si="2"/>
+        <v>12195.532892561983</v>
       </c>
       <c r="I86" s="23">
         <v>2018</v>
@@ -5135,8 +5101,8 @@
       <c r="L86" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="M86" s="23" t="s">
-        <v>92</v>
+      <c r="M86" s="28" t="s">
+        <v>93</v>
       </c>
       <c r="N86" s="23" t="s">
         <v>59</v>
@@ -5144,30 +5110,31 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="23" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B87" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C87" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D87" s="29">
-        <v>37213746</v>
+        <v>60</v>
+      </c>
+      <c r="D87" s="24">
+        <v>36891487</v>
       </c>
       <c r="E87" s="24">
         <f t="shared" si="3"/>
-        <v>3721374.6</v>
+        <v>3689148.7</v>
       </c>
       <c r="F87" s="24">
-        <v>6344</v>
+        <v>3505164</v>
       </c>
       <c r="G87" s="24">
-        <v>634.4</v>
+        <f t="shared" si="4"/>
+        <v>350516.4</v>
       </c>
       <c r="H87" s="25">
-        <f t="shared" si="5"/>
-        <v>5865.975094577554</v>
+        <f t="shared" si="2"/>
+        <v>10.524896124689173</v>
       </c>
       <c r="I87" s="23">
         <v>2018</v>
@@ -5181,8 +5148,8 @@
       <c r="L87" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="M87" s="23" t="s">
-        <v>92</v>
+      <c r="M87" s="28" t="s">
+        <v>93</v>
       </c>
       <c r="N87" s="23" t="s">
         <v>59</v>
@@ -5190,30 +5157,30 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="23" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B88" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C88" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="D88" s="29">
-        <v>37213746</v>
+        <v>22</v>
+      </c>
+      <c r="D88" s="24">
+        <v>36891487</v>
       </c>
       <c r="E88" s="24">
         <f t="shared" si="3"/>
-        <v>3721374.6</v>
+        <v>3689148.7</v>
       </c>
       <c r="F88" s="24">
-        <v>6160965</v>
+        <v>275309.60447761195</v>
       </c>
       <c r="G88" s="24">
-        <v>616096.5</v>
+        <f t="shared" si="4"/>
+        <v>27530.960447761194</v>
       </c>
       <c r="H88" s="25">
-        <f t="shared" si="5"/>
-        <v>6.0402462925856586</v>
+        <v>134</v>
       </c>
       <c r="I88" s="23">
         <v>2018</v>
@@ -5227,8 +5194,8 @@
       <c r="L88" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="M88" s="23" t="s">
-        <v>92</v>
+      <c r="M88" s="28" t="s">
+        <v>93</v>
       </c>
       <c r="N88" s="23" t="s">
         <v>59</v>
@@ -5242,7 +5209,7 @@
         <v>56</v>
       </c>
       <c r="C89" s="23" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D89" s="29">
         <v>37213746</v>
@@ -5252,152 +5219,152 @@
         <v>3721374.6</v>
       </c>
       <c r="F89" s="24">
+        <v>1775985</v>
+      </c>
+      <c r="G89" s="24">
+        <v>177598.5</v>
+      </c>
+      <c r="H89" s="25">
+        <f t="shared" ref="H89:H112" si="5">E89/G89</f>
+        <v>20.95386278600326</v>
+      </c>
+      <c r="I89" s="23">
+        <v>2018</v>
+      </c>
+      <c r="J89" s="23">
+        <v>2027</v>
+      </c>
+      <c r="K89" s="23">
+        <v>2015</v>
+      </c>
+      <c r="L89" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="M89" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="N89" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A90" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C90" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D90" s="29">
+        <v>37213746</v>
+      </c>
+      <c r="E90" s="24">
+        <f t="shared" si="3"/>
+        <v>3721374.6</v>
+      </c>
+      <c r="F90" s="24">
+        <v>6344</v>
+      </c>
+      <c r="G90" s="24">
+        <v>634.4</v>
+      </c>
+      <c r="H90" s="25">
+        <f t="shared" si="5"/>
+        <v>5865.975094577554</v>
+      </c>
+      <c r="I90" s="23">
+        <v>2018</v>
+      </c>
+      <c r="J90" s="23">
+        <v>2027</v>
+      </c>
+      <c r="K90" s="23">
+        <v>2015</v>
+      </c>
+      <c r="L90" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="M90" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="N90" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A91" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C91" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D91" s="29">
+        <v>37213746</v>
+      </c>
+      <c r="E91" s="24">
+        <f t="shared" si="3"/>
+        <v>3721374.6</v>
+      </c>
+      <c r="F91" s="24">
+        <v>6160965</v>
+      </c>
+      <c r="G91" s="24">
+        <v>616096.5</v>
+      </c>
+      <c r="H91" s="25">
+        <f t="shared" si="5"/>
+        <v>6.0402462925856586</v>
+      </c>
+      <c r="I91" s="23">
+        <v>2018</v>
+      </c>
+      <c r="J91" s="23">
+        <v>2027</v>
+      </c>
+      <c r="K91" s="23">
+        <v>2015</v>
+      </c>
+      <c r="L91" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="M91" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="N91" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A92" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B92" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C92" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D92" s="29">
+        <v>37213746</v>
+      </c>
+      <c r="E92" s="24">
+        <f t="shared" si="3"/>
+        <v>3721374.6</v>
+      </c>
+      <c r="F92" s="24">
         <v>333802.36979166669</v>
       </c>
-      <c r="G89" s="24">
+      <c r="G92" s="24">
         <v>33380.236979166672</v>
       </c>
-      <c r="H89" s="25">
+      <c r="H92" s="25">
         <f t="shared" si="5"/>
         <v>111.48436730160395</v>
-      </c>
-      <c r="I89" s="23">
-        <v>2018</v>
-      </c>
-      <c r="J89" s="23">
-        <v>2027</v>
-      </c>
-      <c r="K89" s="23">
-        <v>2015</v>
-      </c>
-      <c r="L89" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="M89" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="N89" s="23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A90" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B90" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C90" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="D90" s="29">
-        <v>73903636</v>
-      </c>
-      <c r="E90" s="24">
-        <f t="shared" si="3"/>
-        <v>7390363.5999999996</v>
-      </c>
-      <c r="F90" s="26">
-        <v>3225501</v>
-      </c>
-      <c r="G90" s="24">
-        <v>322550.09999999998</v>
-      </c>
-      <c r="H90" s="25">
-        <f t="shared" si="5"/>
-        <v>22.912296725376926</v>
-      </c>
-      <c r="I90" s="23">
-        <v>2018</v>
-      </c>
-      <c r="J90" s="23">
-        <v>2027</v>
-      </c>
-      <c r="K90" s="23">
-        <v>2015</v>
-      </c>
-      <c r="L90" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="M90" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="N90" s="23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A91" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B91" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C91" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D91" s="29">
-        <v>73903636</v>
-      </c>
-      <c r="E91" s="24">
-        <f t="shared" si="3"/>
-        <v>7390363.5999999996</v>
-      </c>
-      <c r="F91" s="26">
-        <v>8877</v>
-      </c>
-      <c r="G91" s="24">
-        <v>887.7</v>
-      </c>
-      <c r="H91" s="25">
-        <f t="shared" si="5"/>
-        <v>8325.294130900078</v>
-      </c>
-      <c r="I91" s="23">
-        <v>2018</v>
-      </c>
-      <c r="J91" s="23">
-        <v>2027</v>
-      </c>
-      <c r="K91" s="23">
-        <v>2015</v>
-      </c>
-      <c r="L91" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="M91" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="N91" s="23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A92" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B92" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C92" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="D92" s="29">
-        <v>73903636</v>
-      </c>
-      <c r="E92" s="24">
-        <f t="shared" si="3"/>
-        <v>7390363.5999999996</v>
-      </c>
-      <c r="F92" s="26">
-        <v>8233918</v>
-      </c>
-      <c r="G92" s="24">
-        <v>823391.8</v>
-      </c>
-      <c r="H92" s="25">
-        <f t="shared" si="5"/>
-        <v>8.9755127510378401</v>
       </c>
       <c r="I92" s="23">
         <v>2018</v>
@@ -5426,7 +5393,7 @@
         <v>56</v>
       </c>
       <c r="C93" s="23" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D93" s="29">
         <v>73903636</v>
@@ -5435,15 +5402,15 @@
         <f t="shared" si="3"/>
         <v>7390363.5999999996</v>
       </c>
-      <c r="F93" s="24">
-        <v>416364.65017667843</v>
+      <c r="F93" s="26">
+        <v>3225501</v>
       </c>
       <c r="G93" s="24">
-        <v>41636.465017667841</v>
+        <v>322550.09999999998</v>
       </c>
       <c r="H93" s="25">
         <f t="shared" si="5"/>
-        <v>177.49738352821268</v>
+        <v>22.912296725376926</v>
       </c>
       <c r="I93" s="23">
         <v>2018</v>
@@ -5466,30 +5433,30 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="23" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B94" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C94" s="23" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D94" s="29">
-        <v>1761981734</v>
+        <v>73903636</v>
       </c>
       <c r="E94" s="24">
         <f t="shared" si="3"/>
-        <v>176198173.40000001</v>
-      </c>
-      <c r="F94" s="24">
-        <v>46083379</v>
+        <v>7390363.5999999996</v>
+      </c>
+      <c r="F94" s="26">
+        <v>8877</v>
       </c>
       <c r="G94" s="24">
-        <v>4608337.9000000004</v>
+        <v>887.7</v>
       </c>
       <c r="H94" s="25">
         <f t="shared" si="5"/>
-        <v>38.234647116479891</v>
+        <v>8325.294130900078</v>
       </c>
       <c r="I94" s="23">
         <v>2018</v>
@@ -5512,30 +5479,30 @@
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="23" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B95" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C95" s="23" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D95" s="29">
-        <v>1761981734</v>
+        <v>73903636</v>
       </c>
       <c r="E95" s="24">
         <f t="shared" si="3"/>
-        <v>176198173.40000001</v>
-      </c>
-      <c r="F95" s="24">
-        <v>106007</v>
+        <v>7390363.5999999996</v>
+      </c>
+      <c r="F95" s="26">
+        <v>8233918</v>
       </c>
       <c r="G95" s="24">
-        <v>10600.7</v>
+        <v>823391.8</v>
       </c>
       <c r="H95" s="25">
         <f t="shared" si="5"/>
-        <v>16621.371550935313</v>
+        <v>8.9755127510378401</v>
       </c>
       <c r="I95" s="23">
         <v>2018</v>
@@ -5558,30 +5525,30 @@
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="23" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B96" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C96" s="23" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="D96" s="29">
-        <v>1761981734</v>
+        <v>73903636</v>
       </c>
       <c r="E96" s="24">
         <f t="shared" si="3"/>
-        <v>176198173.40000001</v>
+        <v>7390363.5999999996</v>
       </c>
       <c r="F96" s="24">
-        <v>117772708</v>
+        <v>416364.65017667843</v>
       </c>
       <c r="G96" s="24">
-        <v>11777270.800000001</v>
+        <v>41636.465017667841</v>
       </c>
       <c r="H96" s="25">
         <f t="shared" si="5"/>
-        <v>14.960866264533884</v>
+        <v>177.49738352821268</v>
       </c>
       <c r="I96" s="23">
         <v>2018</v>
@@ -5610,7 +5577,7 @@
         <v>56</v>
       </c>
       <c r="C97" s="23" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D97" s="29">
         <v>1761981734</v>
@@ -5620,14 +5587,14 @@
         <v>176198173.40000001</v>
       </c>
       <c r="F97" s="24">
-        <v>2996567.5748299318</v>
+        <v>46083379</v>
       </c>
       <c r="G97" s="24">
-        <v>299656.75748299318</v>
+        <v>4608337.9000000004</v>
       </c>
       <c r="H97" s="25">
         <f t="shared" si="5"/>
-        <v>588</v>
+        <v>38.234647116479891</v>
       </c>
       <c r="I97" s="23">
         <v>2018</v>
@@ -5650,30 +5617,30 @@
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B98" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C98" s="23" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D98" s="29">
-        <v>287705916</v>
+        <v>1761981734</v>
       </c>
       <c r="E98" s="24">
         <f t="shared" si="3"/>
-        <v>28770591.600000001</v>
+        <v>176198173.40000001</v>
       </c>
       <c r="F98" s="24">
-        <v>10650771</v>
+        <v>106007</v>
       </c>
       <c r="G98" s="24">
-        <v>1065077.1000000001</v>
+        <v>10600.7</v>
       </c>
       <c r="H98" s="25">
         <f t="shared" si="5"/>
-        <v>27.012684433831126</v>
+        <v>16621.371550935313</v>
       </c>
       <c r="I98" s="23">
         <v>2018</v>
@@ -5696,30 +5663,30 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B99" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C99" s="23" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D99" s="29">
-        <v>287705916</v>
+        <v>1761981734</v>
       </c>
       <c r="E99" s="24">
         <f t="shared" si="3"/>
-        <v>28770591.600000001</v>
+        <v>176198173.40000001</v>
       </c>
       <c r="F99" s="24">
-        <v>91934</v>
+        <v>117772708</v>
       </c>
       <c r="G99" s="24">
-        <v>9193.4</v>
+        <v>11777270.800000001</v>
       </c>
       <c r="H99" s="25">
         <f t="shared" si="5"/>
-        <v>3129.4832814845436</v>
+        <v>14.960866264533884</v>
       </c>
       <c r="I99" s="23">
         <v>2018</v>
@@ -5742,30 +5709,30 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B100" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C100" s="23" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="D100" s="29">
-        <v>287705916</v>
+        <v>1761981734</v>
       </c>
       <c r="E100" s="24">
         <f t="shared" si="3"/>
-        <v>28770591.600000001</v>
+        <v>176198173.40000001</v>
       </c>
       <c r="F100" s="24">
-        <v>28485738</v>
+        <v>2996567.5748299318</v>
       </c>
       <c r="G100" s="24">
-        <v>2848573.8</v>
+        <v>299656.75748299318</v>
       </c>
       <c r="H100" s="25">
         <f t="shared" si="5"/>
-        <v>10.099998673020163</v>
+        <v>588</v>
       </c>
       <c r="I100" s="23">
         <v>2018</v>
@@ -5794,7 +5761,7 @@
         <v>56</v>
       </c>
       <c r="C101" s="23" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D101" s="29">
         <v>287705916</v>
@@ -5804,14 +5771,14 @@
         <v>28770591.600000001</v>
       </c>
       <c r="F101" s="24">
-        <v>2950264.3448275863</v>
+        <v>10650771</v>
       </c>
       <c r="G101" s="24">
-        <v>295026.43448275863</v>
+        <v>1065077.1000000001</v>
       </c>
       <c r="H101" s="25">
         <f t="shared" si="5"/>
-        <v>97.518690657129426</v>
+        <v>27.012684433831126</v>
       </c>
       <c r="I101" s="23">
         <v>2018</v>
@@ -5834,30 +5801,30 @@
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="23" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B102" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C102" s="23" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D102" s="29">
-        <v>77669464</v>
+        <v>287705916</v>
       </c>
       <c r="E102" s="24">
         <f t="shared" si="3"/>
-        <v>7766946.4000000004</v>
+        <v>28770591.600000001</v>
       </c>
       <c r="F102" s="24">
-        <v>2242237</v>
+        <v>91934</v>
       </c>
       <c r="G102" s="24">
-        <v>224223.7</v>
+        <v>9193.4</v>
       </c>
       <c r="H102" s="25">
         <f t="shared" si="5"/>
-        <v>34.639274974054928</v>
+        <v>3129.4832814845436</v>
       </c>
       <c r="I102" s="23">
         <v>2018</v>
@@ -5880,30 +5847,30 @@
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="23" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B103" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C103" s="23" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D103" s="29">
-        <v>77669464</v>
+        <v>287705916</v>
       </c>
       <c r="E103" s="24">
         <f t="shared" si="3"/>
-        <v>7766946.4000000004</v>
+        <v>28770591.600000001</v>
       </c>
       <c r="F103" s="24">
-        <v>30528</v>
+        <v>28485738</v>
       </c>
       <c r="G103" s="24">
-        <v>3052.8</v>
+        <v>2848573.8</v>
       </c>
       <c r="H103" s="25">
         <f t="shared" si="5"/>
-        <v>2544.204140461216</v>
+        <v>10.099998673020163</v>
       </c>
       <c r="I103" s="23">
         <v>2018</v>
@@ -5926,30 +5893,30 @@
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="23" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B104" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C104" s="23" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="D104" s="29">
-        <v>77669464</v>
+        <v>287705916</v>
       </c>
       <c r="E104" s="24">
         <f t="shared" si="3"/>
-        <v>7766946.4000000004</v>
+        <v>28770591.600000001</v>
       </c>
       <c r="F104" s="24">
-        <v>21333511</v>
+        <v>2950264.3448275863</v>
       </c>
       <c r="G104" s="24">
-        <v>2133351.1</v>
+        <v>295026.43448275863</v>
       </c>
       <c r="H104" s="25">
         <f t="shared" si="5"/>
-        <v>3.6407258045804087</v>
+        <v>97.518690657129426</v>
       </c>
       <c r="I104" s="23">
         <v>2018</v>
@@ -5978,7 +5945,7 @@
         <v>56</v>
       </c>
       <c r="C105" s="23" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D105" s="29">
         <v>77669464</v>
@@ -5988,14 +5955,14 @@
         <v>7766946.4000000004</v>
       </c>
       <c r="F105" s="24">
-        <v>1049587.3513513512</v>
+        <v>2242237</v>
       </c>
       <c r="G105" s="24">
-        <v>104958.73513513512</v>
+        <v>224223.7</v>
       </c>
       <c r="H105" s="25">
         <f t="shared" si="5"/>
-        <v>74.000000000000014</v>
+        <v>34.639274974054928</v>
       </c>
       <c r="I105" s="23">
         <v>2018</v>
@@ -6018,30 +5985,30 @@
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="23" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B106" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C106" s="23" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D106" s="29">
-        <v>14096578</v>
+        <v>77669464</v>
       </c>
       <c r="E106" s="24">
         <f t="shared" si="3"/>
-        <v>1409657.8</v>
+        <v>7766946.4000000004</v>
       </c>
       <c r="F106" s="24">
-        <v>1078428</v>
+        <v>30528</v>
       </c>
       <c r="G106" s="24">
-        <v>107842.8</v>
+        <v>3052.8</v>
       </c>
       <c r="H106" s="25">
         <f t="shared" si="5"/>
-        <v>13.071413205146751</v>
+        <v>2544.204140461216</v>
       </c>
       <c r="I106" s="23">
         <v>2018</v>
@@ -6064,30 +6031,30 @@
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="23" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B107" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C107" s="23" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D107" s="29">
-        <v>14096578</v>
+        <v>77669464</v>
       </c>
       <c r="E107" s="24">
         <f t="shared" si="3"/>
-        <v>1409657.8</v>
+        <v>7766946.4000000004</v>
       </c>
       <c r="F107" s="24">
-        <v>3025</v>
+        <v>21333511</v>
       </c>
       <c r="G107" s="24">
-        <v>302.5</v>
+        <v>2133351.1</v>
       </c>
       <c r="H107" s="25">
         <f t="shared" si="5"/>
-        <v>4660.0257851239667</v>
+        <v>3.6407258045804087</v>
       </c>
       <c r="I107" s="23">
         <v>2018</v>
@@ -6110,30 +6077,30 @@
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="23" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B108" s="23" t="s">
         <v>56</v>
       </c>
       <c r="C108" s="23" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="D108" s="29">
-        <v>14096578</v>
+        <v>77669464</v>
       </c>
       <c r="E108" s="24">
         <f t="shared" si="3"/>
-        <v>1409657.8</v>
+        <v>7766946.4000000004</v>
       </c>
       <c r="F108" s="24">
-        <v>3505164</v>
+        <v>1049587.3513513512</v>
       </c>
       <c r="G108" s="24">
-        <v>350516.4</v>
+        <v>104958.73513513512</v>
       </c>
       <c r="H108" s="25">
         <f t="shared" si="5"/>
-        <v>4.021660042154946</v>
+        <v>74.000000000000014</v>
       </c>
       <c r="I108" s="23">
         <v>2018</v>
@@ -6162,7 +6129,7 @@
         <v>56</v>
       </c>
       <c r="C109" s="23" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D109" s="29">
         <v>14096578</v>
@@ -6172,14 +6139,14 @@
         <v>1409657.8</v>
       </c>
       <c r="F109" s="24">
-        <v>275309.60447761195</v>
+        <v>1078428</v>
       </c>
       <c r="G109" s="24">
-        <v>27530.960447761194</v>
+        <v>107842.8</v>
       </c>
       <c r="H109" s="25">
         <f t="shared" si="5"/>
-        <v>51.202637941918688</v>
+        <v>13.071413205146751</v>
       </c>
       <c r="I109" s="23">
         <v>2018</v>
@@ -6197,6 +6164,144 @@
         <v>92</v>
       </c>
       <c r="N109" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A110" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B110" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C110" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D110" s="29">
+        <v>14096578</v>
+      </c>
+      <c r="E110" s="24">
+        <f t="shared" si="3"/>
+        <v>1409657.8</v>
+      </c>
+      <c r="F110" s="24">
+        <v>3025</v>
+      </c>
+      <c r="G110" s="24">
+        <v>302.5</v>
+      </c>
+      <c r="H110" s="25">
+        <f t="shared" si="5"/>
+        <v>4660.0257851239667</v>
+      </c>
+      <c r="I110" s="23">
+        <v>2018</v>
+      </c>
+      <c r="J110" s="23">
+        <v>2027</v>
+      </c>
+      <c r="K110" s="23">
+        <v>2015</v>
+      </c>
+      <c r="L110" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="M110" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="N110" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A111" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B111" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C111" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D111" s="29">
+        <v>14096578</v>
+      </c>
+      <c r="E111" s="24">
+        <f t="shared" si="3"/>
+        <v>1409657.8</v>
+      </c>
+      <c r="F111" s="24">
+        <v>3505164</v>
+      </c>
+      <c r="G111" s="24">
+        <v>350516.4</v>
+      </c>
+      <c r="H111" s="25">
+        <f t="shared" si="5"/>
+        <v>4.021660042154946</v>
+      </c>
+      <c r="I111" s="23">
+        <v>2018</v>
+      </c>
+      <c r="J111" s="23">
+        <v>2027</v>
+      </c>
+      <c r="K111" s="23">
+        <v>2015</v>
+      </c>
+      <c r="L111" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="M111" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="N111" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A112" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B112" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C112" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D112" s="29">
+        <v>14096578</v>
+      </c>
+      <c r="E112" s="24">
+        <f t="shared" si="3"/>
+        <v>1409657.8</v>
+      </c>
+      <c r="F112" s="24">
+        <v>275309.60447761195</v>
+      </c>
+      <c r="G112" s="24">
+        <v>27530.960447761194</v>
+      </c>
+      <c r="H112" s="25">
+        <f t="shared" si="5"/>
+        <v>51.202637941918688</v>
+      </c>
+      <c r="I112" s="23">
+        <v>2018</v>
+      </c>
+      <c r="J112" s="23">
+        <v>2027</v>
+      </c>
+      <c r="K112" s="23">
+        <v>2015</v>
+      </c>
+      <c r="L112" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="M112" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="N112" s="23" t="s">
         <v>59</v>
       </c>
     </row>
@@ -6210,8 +6315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6651,7 +6756,7 @@
         <v>8439500</v>
       </c>
       <c r="G15" s="18">
-        <f t="shared" ref="G15:G37" si="1">E15/D15*100</f>
+        <f t="shared" ref="G15:G36" si="1">E15/D15*100</f>
         <v>6.396627860742317</v>
       </c>
       <c r="H15" s="17">

</xml_diff>